<commit_message>
Improve note book and handling of partnerCode=None
</commit_message>
<xml_diff>
--- a/reports/Angola_export_top_5_partners_2003-2022.xlsx
+++ b/reports/Angola_export_top_5_partners_2003-2022.xlsx
@@ -2319,40 +2319,40 @@
         <v>19</v>
       </c>
       <c r="C23">
-        <v>0.0009268444316100792</v>
+        <v>0.0009268444936706236</v>
       </c>
       <c r="D23">
-        <v>0.007982777548225989</v>
+        <v>0.007982778082744516</v>
       </c>
       <c r="E23">
-        <v>0.4755840503137769</v>
+        <v>0.4755840821583929</v>
       </c>
       <c r="F23">
-        <v>0.08009449841450408</v>
+        <v>0.08009450377754884</v>
       </c>
       <c r="G23">
-        <v>0.07717931158014271</v>
+        <v>0.07717931674798957</v>
       </c>
       <c r="H23">
-        <v>0.10019201178242</v>
+        <v>0.1001920184911734</v>
       </c>
       <c r="J23">
-        <v>0.01344400552977868</v>
+        <v>0.01344400642997538</v>
       </c>
       <c r="K23">
-        <v>1.387114093462033E-05</v>
+        <v>1.387114186341758E-05</v>
       </c>
       <c r="L23">
-        <v>0.009752239384306473</v>
+        <v>0.009752240037306334</v>
       </c>
       <c r="M23">
-        <v>0.04276267534630596</v>
+        <v>0.04276267820965047</v>
       </c>
       <c r="O23">
-        <v>0.03354605567950121</v>
+        <v>0.03354605792571039</v>
       </c>
       <c r="P23">
-        <v>0.04073309370597102</v>
+        <v>0.04073309643341684</v>
       </c>
       <c r="Q23">
         <v>45303062.078</v>

</xml_diff>